<commit_message>
Analise de Previsão - Modelo Amort_Exponencial
</commit_message>
<xml_diff>
--- a/amortecomentoExpon/fit.xlsx
+++ b/amortecomentoExpon/fit.xlsx
@@ -377,206 +377,206 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>82.9987191435649</v>
+        <v>80.5220498566652</v>
       </c>
       <c r="B2" t="n">
-        <v>75.1913181912349</v>
+        <v>72.7148740564601</v>
       </c>
       <c r="C2" t="n">
-        <v>90.8061200958949</v>
+        <v>88.3292256568703</v>
       </c>
       <c r="D2" t="n">
-        <v>71.0583297820741</v>
+        <v>68.5820048356347</v>
       </c>
       <c r="E2" t="n">
-        <v>94.9391085050557</v>
+        <v>92.4620948776958</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>82.9987191435649</v>
+        <v>80.5220498566652</v>
       </c>
       <c r="B3" t="n">
-        <v>73.0003674897207</v>
+        <v>70.5239865382267</v>
       </c>
       <c r="C3" t="n">
-        <v>92.9970707974091</v>
+        <v>90.5201131751037</v>
       </c>
       <c r="D3" t="n">
-        <v>67.7075598385755</v>
+        <v>65.2313315226252</v>
       </c>
       <c r="E3" t="n">
-        <v>98.2898784485543</v>
+        <v>95.8127681907052</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>82.9987191435649</v>
+        <v>80.5220498566652</v>
       </c>
       <c r="B4" t="n">
-        <v>71.2098022315915</v>
+        <v>68.733472916945</v>
       </c>
       <c r="C4" t="n">
-        <v>94.7876360555383</v>
+        <v>92.3106267963854</v>
       </c>
       <c r="D4" t="n">
-        <v>64.9691265891802</v>
+        <v>62.4929772449733</v>
       </c>
       <c r="E4" t="n">
-        <v>101.02831169795</v>
+        <v>98.5511224683571</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>82.9987191435649</v>
+        <v>80.5220498566652</v>
       </c>
       <c r="B5" t="n">
-        <v>69.6574265479842</v>
+        <v>67.1811420012042</v>
       </c>
       <c r="C5" t="n">
-        <v>96.3400117391456</v>
+        <v>93.8629577121262</v>
       </c>
       <c r="D5" t="n">
-        <v>62.5949728585395</v>
+        <v>60.1188919808762</v>
       </c>
       <c r="E5" t="n">
-        <v>103.40246542859</v>
+        <v>100.925207732454</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>82.9987191435649</v>
+        <v>80.5220498566652</v>
       </c>
       <c r="B6" t="n">
-        <v>68.2677444886284</v>
+        <v>65.7915000179084</v>
       </c>
       <c r="C6" t="n">
-        <v>97.7296937985014</v>
+        <v>95.252599695422</v>
       </c>
       <c r="D6" t="n">
-        <v>60.4696375544222</v>
+        <v>57.9936179678035</v>
       </c>
       <c r="E6" t="n">
-        <v>105.527800732708</v>
+        <v>103.050481745527</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>82.9987191435649</v>
+        <v>80.5220498566652</v>
       </c>
       <c r="B7" t="n">
-        <v>66.9983085098385</v>
+        <v>64.5221006474866</v>
       </c>
       <c r="C7" t="n">
-        <v>98.9991297772913</v>
+        <v>96.5219990658438</v>
       </c>
       <c r="D7" t="n">
-        <v>58.5282027608482</v>
+        <v>56.052239161897</v>
       </c>
       <c r="E7" t="n">
-        <v>107.469235526282</v>
+        <v>104.991860551433</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>82.9987191435649</v>
+        <v>80.5220498566652</v>
       </c>
       <c r="B8" t="n">
-        <v>65.8224370484388</v>
+        <v>63.346263096214</v>
       </c>
       <c r="C8" t="n">
-        <v>100.175001238691</v>
+        <v>97.6978366171165</v>
       </c>
       <c r="D8" t="n">
-        <v>56.7298625482852</v>
+        <v>54.253950810398</v>
       </c>
       <c r="E8" t="n">
-        <v>109.267575738845</v>
+        <v>106.790148902932</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>82.9987191435649</v>
+        <v>80.5220498566652</v>
       </c>
       <c r="B9" t="n">
-        <v>64.7220620976269</v>
+        <v>62.2459198783386</v>
       </c>
       <c r="C9" t="n">
-        <v>101.275376189503</v>
+        <v>98.7981798349919</v>
       </c>
       <c r="D9" t="n">
-        <v>55.0469842848852</v>
+        <v>52.5711210783363</v>
       </c>
       <c r="E9" t="n">
-        <v>110.950454002245</v>
+        <v>108.472978634994</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>82.9987191435649</v>
+        <v>80.5220498566652</v>
       </c>
       <c r="B10" t="n">
-        <v>63.6842758707621</v>
+        <v>61.2081635794581</v>
       </c>
       <c r="C10" t="n">
-        <v>102.313162416368</v>
+        <v>99.8359361338723</v>
       </c>
       <c r="D10" t="n">
-        <v>53.4598272145082</v>
+        <v>50.9840097788617</v>
       </c>
       <c r="E10" t="n">
-        <v>112.537611072622</v>
+        <v>110.060089934469</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>82.9987191435649</v>
+        <v>80.5220498566652</v>
       </c>
       <c r="B11" t="n">
-        <v>62.6994766675068</v>
+        <v>60.2233927761319</v>
       </c>
       <c r="C11" t="n">
-        <v>103.297961619623</v>
+        <v>100.820706937199</v>
       </c>
       <c r="D11" t="n">
-        <v>51.9537068036889</v>
+        <v>49.4779328019858</v>
       </c>
       <c r="E11" t="n">
-        <v>114.043731483441</v>
+        <v>111.566166911345</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>82.9987191435649</v>
+        <v>80.5220498566652</v>
       </c>
       <c r="B12" t="n">
-        <v>61.7602923829669</v>
+        <v>59.2842355760646</v>
       </c>
       <c r="C12" t="n">
-        <v>104.237145904163</v>
+        <v>101.759864137266</v>
       </c>
       <c r="D12" t="n">
-        <v>50.5173483909379</v>
+        <v>48.0416158113611</v>
       </c>
       <c r="E12" t="n">
-        <v>115.480089896192</v>
+        <v>113.002483901969</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>82.9987191435649</v>
+        <v>80.5220498566652</v>
       </c>
       <c r="B13" t="n">
-        <v>60.8609166910004</v>
+        <v>58.3848858205589</v>
       </c>
       <c r="C13" t="n">
-        <v>105.136521596129</v>
+        <v>102.659213892772</v>
       </c>
       <c r="D13" t="n">
-        <v>49.1418719667208</v>
+        <v>46.6661790535378</v>
       </c>
       <c r="E13" t="n">
-        <v>116.855566320409</v>
+        <v>114.377920659793</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Metodos de Holt e Holt_Winters
</commit_message>
<xml_diff>
--- a/amortecomentoExpon/fit.xlsx
+++ b/amortecomentoExpon/fit.xlsx
@@ -377,206 +377,206 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>80.5220498566652</v>
+        <v>80.1591730318595</v>
       </c>
       <c r="B2" t="n">
-        <v>72.7148740564601</v>
+        <v>72.3554257855546</v>
       </c>
       <c r="C2" t="n">
-        <v>88.3292256568703</v>
+        <v>87.9629202781644</v>
       </c>
       <c r="D2" t="n">
-        <v>68.5820048356347</v>
+        <v>68.2243715315301</v>
       </c>
       <c r="E2" t="n">
-        <v>92.4620948776958</v>
+        <v>92.0939745321889</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>80.5220498566652</v>
+        <v>80.1591730318595</v>
       </c>
       <c r="B3" t="n">
-        <v>70.5239865382267</v>
+        <v>70.0330370700905</v>
       </c>
       <c r="C3" t="n">
-        <v>90.5201131751037</v>
+        <v>90.2853089936285</v>
       </c>
       <c r="D3" t="n">
-        <v>65.2313315226252</v>
+        <v>64.6725844924517</v>
       </c>
       <c r="E3" t="n">
-        <v>95.8127681907052</v>
+        <v>95.6457615712673</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>80.5220498566652</v>
+        <v>80.1591730318595</v>
       </c>
       <c r="B4" t="n">
-        <v>68.733472916945</v>
+        <v>68.1517258448737</v>
       </c>
       <c r="C4" t="n">
-        <v>92.3106267963854</v>
+        <v>92.1666202188453</v>
       </c>
       <c r="D4" t="n">
-        <v>62.4929772449733</v>
+        <v>61.7953672627503</v>
       </c>
       <c r="E4" t="n">
-        <v>98.5511224683571</v>
+        <v>98.5229788009687</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>80.5220498566652</v>
+        <v>80.1591730318595</v>
       </c>
       <c r="B5" t="n">
-        <v>67.1811420012042</v>
+        <v>66.5276306987164</v>
       </c>
       <c r="C5" t="n">
-        <v>93.8629577121262</v>
+        <v>93.7907153650026</v>
       </c>
       <c r="D5" t="n">
-        <v>60.1188919808762</v>
+        <v>59.3115280794381</v>
       </c>
       <c r="E5" t="n">
-        <v>100.925207732454</v>
+        <v>101.006817984281</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>80.5220498566652</v>
+        <v>80.1591730318595</v>
       </c>
       <c r="B6" t="n">
-        <v>65.7915000179084</v>
+        <v>65.0774256260615</v>
       </c>
       <c r="C6" t="n">
-        <v>95.252599695422</v>
+        <v>95.2409204376575</v>
       </c>
       <c r="D6" t="n">
-        <v>57.9936179678035</v>
+        <v>57.0936308141081</v>
       </c>
       <c r="E6" t="n">
-        <v>103.050481745527</v>
+        <v>103.224715249611</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>80.5220498566652</v>
+        <v>80.1591730318595</v>
       </c>
       <c r="B7" t="n">
-        <v>64.5221006474866</v>
+        <v>63.7549277507039</v>
       </c>
       <c r="C7" t="n">
-        <v>96.5219990658438</v>
+        <v>96.5634183130151</v>
       </c>
       <c r="D7" t="n">
-        <v>56.052239161897</v>
+        <v>55.0710448526683</v>
       </c>
       <c r="E7" t="n">
-        <v>104.991860551433</v>
+        <v>105.247301211051</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>80.5220498566652</v>
+        <v>80.1591730318595</v>
       </c>
       <c r="B8" t="n">
-        <v>63.346263096214</v>
+        <v>62.5313705120802</v>
       </c>
       <c r="C8" t="n">
-        <v>97.6978366171165</v>
+        <v>97.7869755516388</v>
       </c>
       <c r="D8" t="n">
-        <v>54.253950810398</v>
+        <v>53.1997755372533</v>
       </c>
       <c r="E8" t="n">
-        <v>106.790148902932</v>
+        <v>107.118570526466</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>80.5220498566652</v>
+        <v>80.1591730318595</v>
       </c>
       <c r="B9" t="n">
-        <v>62.2459198783386</v>
+        <v>61.387396874331</v>
       </c>
       <c r="C9" t="n">
-        <v>98.7981798349919</v>
+        <v>98.930949189388</v>
       </c>
       <c r="D9" t="n">
-        <v>52.5711210783363</v>
+        <v>51.4502188361938</v>
       </c>
       <c r="E9" t="n">
-        <v>108.472978634994</v>
+        <v>108.868127227525</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>80.5220498566652</v>
+        <v>80.1591730318595</v>
       </c>
       <c r="B10" t="n">
-        <v>61.2081635794581</v>
+        <v>60.3092425901583</v>
       </c>
       <c r="C10" t="n">
-        <v>99.8359361338723</v>
+        <v>100.009103473561</v>
       </c>
       <c r="D10" t="n">
-        <v>50.9840097788617</v>
+        <v>49.8013241498079</v>
       </c>
       <c r="E10" t="n">
-        <v>110.060089934469</v>
+        <v>110.517021913911</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>80.5220498566652</v>
+        <v>80.1591730318595</v>
       </c>
       <c r="B11" t="n">
-        <v>60.2233927761319</v>
+        <v>59.2867055933318</v>
       </c>
       <c r="C11" t="n">
-        <v>100.820706937199</v>
+        <v>101.031640470387</v>
       </c>
       <c r="D11" t="n">
-        <v>49.4779328019858</v>
+        <v>48.2374887642314</v>
       </c>
       <c r="E11" t="n">
-        <v>111.566166911345</v>
+        <v>112.080857299488</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>80.5220498566652</v>
+        <v>80.1591730318595</v>
       </c>
       <c r="B12" t="n">
-        <v>59.2842355760646</v>
+        <v>58.3119751473614</v>
       </c>
       <c r="C12" t="n">
-        <v>101.759864137266</v>
+        <v>102.006370916358</v>
       </c>
       <c r="D12" t="n">
-        <v>48.0416158113611</v>
+        <v>46.7467671888378</v>
       </c>
       <c r="E12" t="n">
-        <v>113.002483901969</v>
+        <v>113.571578874881</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>80.5220498566652</v>
+        <v>80.1591730318595</v>
       </c>
       <c r="B13" t="n">
-        <v>58.3848858205589</v>
+        <v>57.3789137305161</v>
       </c>
       <c r="C13" t="n">
-        <v>102.659213892772</v>
+        <v>102.939432333203</v>
       </c>
       <c r="D13" t="n">
-        <v>46.6661790535378</v>
+        <v>45.3197728941499</v>
       </c>
       <c r="E13" t="n">
-        <v>114.377920659793</v>
+        <v>114.998573169569</v>
       </c>
     </row>
   </sheetData>

</xml_diff>